<commit_message>
v2.95 Falta actualizar contraseña
</commit_message>
<xml_diff>
--- a/Unit test.xlsx
+++ b/Unit test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="88">
   <si>
     <t>Nombre del proyecto:</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t xml:space="preserve">La imagen se sube correctamente, pero no sustituye la imagen anterior </t>
+  </si>
+  <si>
+    <t>Borrar el avatar anterior antes de cargar el avatar nuevo</t>
   </si>
   <si>
     <t>27/8</t>
@@ -1431,9 +1434,11 @@
       <c r="E21" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="9"/>
+      <c r="F21" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="G21" s="6" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -1460,16 +1465,16 @@
         <v>16.0</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="6" t="s">
@@ -1500,13 +1505,13 @@
         <v>17.0</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>21</v>
@@ -1540,13 +1545,13 @@
         <v>18.0</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>21</v>
@@ -1580,13 +1585,13 @@
         <v>19.0</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>21</v>
@@ -1620,13 +1625,13 @@
         <v>20.0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>21</v>
@@ -1663,10 +1668,10 @@
         <v>44660.0</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>21</v>
@@ -1703,10 +1708,10 @@
         <v>44660.0</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>21</v>
@@ -1736,11 +1741,11 @@
       <c r="Z28" s="3"/>
     </row>
     <row r="29" ht="37.5" customHeight="1">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
       <c r="F29" s="9"/>
       <c r="G29" s="6"/>
       <c r="H29" s="3"/>

</xml_diff>